<commit_message>
Updated the Query Request sample
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Wildlife_License_Query_Request/artifacts/service_model/information_model/IEPD/documentation/Wildlife_License_Query_Request.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Wildlife_License_Query_Request/artifacts/service_model/information_model/IEPD/documentation/Wildlife_License_Query_Request.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="1520" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="-26880" yWindow="1520" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="eCitation" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-  </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,7 +243,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="730">
+  <cellStyleXfs count="732">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -977,8 +974,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -993,9 +992,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1014,7 +1010,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="730">
+  <cellStyles count="732">
     <cellStyle name="Accent1 - 20%" xfId="3"/>
     <cellStyle name="Accent1 - 40%" xfId="4"/>
     <cellStyle name="Accent1 - 60%" xfId="5"/>
@@ -1388,6 +1384,7 @@
     <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
@@ -1740,6 +1737,7 @@
     <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="24"/>
@@ -2043,11 +2041,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2059,32 +2057,32 @@
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="15">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2101,16 +2099,12 @@
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1">
       <c r="A5" s="4"/>
-      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1">
       <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1">
       <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" s="2" customFormat="1">
-      <c r="A8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>